<commit_message>
Minor fixes here and there.
</commit_message>
<xml_diff>
--- a/resources/data-imports/npcs.xlsx
+++ b/resources/data-imports/npcs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
   <si>
     <t>name</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>DungeonMaiden</t>
-  </si>
-  <si>
-    <t>Dungeon Maiden</t>
   </si>
   <si>
     <t>Dungeons</t>
@@ -689,25 +686,25 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
         <v>31</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>32</v>
-      </c>
       <c r="H8">
-        <v>128</v>
+        <v>448</v>
       </c>
       <c r="I8">
-        <v>432</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -746,13 +743,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -760,7 +757,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -771,7 +768,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -782,7 +779,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -793,7 +790,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -804,7 +801,7 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -815,7 +812,7 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -823,10 +820,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8">
         <v>2</v>

</xml_diff>

<commit_message>
Added new quest items, npc and quest.
- Finished adding 15 new monsters to each plane.
- Added Devouring Light and Devouring Darkness to Items, for quest
  items.
- Updated items page to show the quest the item comes from or came from.
- Added new help doc for voidance.
- Enemies can already void, but now lets put devoid and void in place
  for characters
</commit_message>
<xml_diff>
--- a/resources/data-imports/npcs.xlsx
+++ b/resources/data-imports/npcs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <t>name</t>
   </si>
@@ -114,6 +114,15 @@
     <t>/m DungeonMaiden:</t>
   </si>
   <si>
+    <t>WonderingMerchant</t>
+  </si>
+  <si>
+    <t>Wondering Merchant</t>
+  </si>
+  <si>
+    <t>/m WonderingMerchant:</t>
+  </si>
+  <si>
     <t>npc_id</t>
   </si>
   <si>
@@ -142,6 +151,9 @@
   </si>
   <si>
     <t>Summon</t>
+  </si>
+  <si>
+    <t>Voidance</t>
   </si>
 </sst>
 </file>
@@ -480,7 +492,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,8 +500,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="19" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="21" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="22" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="5" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="19" bestFit="true" customWidth="true" style="0"/>
@@ -705,6 +717,32 @@
       </c>
       <c r="I8">
         <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9">
+        <v>32</v>
+      </c>
+      <c r="I9">
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -728,7 +766,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -736,20 +774,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="22" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="16" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="15" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -757,7 +795,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -768,7 +806,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -779,7 +817,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -790,7 +828,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -801,7 +839,7 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -812,7 +850,7 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -823,10 +861,21 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C8">
         <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
We can now level past level 1000
</commit_message>
<xml_diff>
--- a/resources/data-imports/npcs.xlsx
+++ b/resources/data-imports/npcs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>name</t>
   </si>
@@ -123,6 +123,15 @@
     <t>/m WonderingMerchant:</t>
   </si>
   <si>
+    <t>LabyrinthWeaver</t>
+  </si>
+  <si>
+    <t>Labyrinth Weaver</t>
+  </si>
+  <si>
+    <t>/m LabyrinthWeaver:</t>
+  </si>
+  <si>
     <t>npc_id</t>
   </si>
   <si>
@@ -154,6 +163,9 @@
   </si>
   <si>
     <t>Voidance</t>
+  </si>
+  <si>
+    <t>Make Sash</t>
   </si>
 </sst>
 </file>
@@ -492,7 +504,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -745,6 +757,32 @@
         <v>256</v>
       </c>
     </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10">
+        <v>384</v>
+      </c>
+      <c r="I10">
+        <v>496</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
@@ -766,7 +804,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -781,13 +819,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -795,7 +833,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -806,7 +844,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -817,7 +855,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -828,7 +866,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -839,7 +877,7 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -850,7 +888,7 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -861,7 +899,7 @@
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -872,9 +910,20 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10">
         <v>0</v>
       </c>
     </row>

</xml_diff>